<commit_message>
Renamed sheet, deleted file
</commit_message>
<xml_diff>
--- a/Training Dataset Wkbk.xlsx
+++ b/Training Dataset Wkbk.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DhruvGupta/Desktop/3B/MSCI 446/MSCI446-TwitterStockMining/MSCI446-TwitterStockMining/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MattC/Documents/School/3B/MSCI 446 Data Mining/Project/MSCI446-TwitterStockMining/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Training Dataset" sheetId="1" r:id="rId1"/>
     <sheet name="Clean Training Dataset" sheetId="8" r:id="rId2"/>
-    <sheet name="Clean Training Dataset (2)" sheetId="13" r:id="rId3"/>
+    <sheet name="CSV" sheetId="13" r:id="rId3"/>
     <sheet name="Normalization Factors" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Clean Training Dataset'!$A$4:$AC$85</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Clean Training Dataset (2)'!$A$2:$K$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CSV!$A$2:$K$83</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -11016,11 +11016,11 @@
         <v>49.4</v>
       </c>
       <c r="AA100" s="4">
-        <f t="shared" ref="AA100:AA131" si="47">IFERROR((Z100-Y100)/Y100, "N/A")</f>
+        <f t="shared" ref="AA100:AA116" si="47">IFERROR((Z100-Y100)/Y100, "N/A")</f>
         <v>6.1099796334011637E-3</v>
       </c>
       <c r="AB100" t="str">
-        <f t="shared" ref="AB100:AB131" si="48">IF(AA100="N/A", "N/A", IF(AA100&gt;0, "UP", "DOWN"))</f>
+        <f t="shared" ref="AB100:AB116" si="48">IF(AA100="N/A", "N/A", IF(AA100&gt;0, "UP", "DOWN"))</f>
         <v>UP</v>
       </c>
       <c r="AC100">
@@ -19906,11 +19906,11 @@
         <v>84.27</v>
       </c>
       <c r="AA68" s="4">
-        <f t="shared" ref="AA68:AA99" si="35">IFERROR((Z68-Y68)/Y68, "N/A")</f>
+        <f t="shared" ref="AA68:AA85" si="35">IFERROR((Z68-Y68)/Y68, "N/A")</f>
         <v>-5.8983130824584173E-3</v>
       </c>
       <c r="AB68" t="str">
-        <f t="shared" ref="AB68:AB99" si="36">IF(AA68="N/A", "N/A", IF(AA68&gt;0, "UP", "DOWN"))</f>
+        <f t="shared" ref="AB68:AB85" si="36">IF(AA68="N/A", "N/A", IF(AA68&gt;0, "UP", "DOWN"))</f>
         <v>DOWN</v>
       </c>
       <c r="AC68">

</xml_diff>